<commit_message>
(hel-884) Correction du wording sur le taux de vétusté de constructions
</commit_message>
<xml_diff>
--- a/public/templates/template_comparaison_MS.xlsx
+++ b/public/templates/template_comparaison_MS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\webadm\projets\helios\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://catamaniacrm-my.sharepoint.com/personal/y_elhouakmi_catamania_com/Documents/Documents/DNum/Helios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{F079C0BB-4954-401D-98BD-E461652969BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D29013A-4563-4221-BE0D-8043D3372986}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{F079C0BB-4954-401D-98BD-E461652969BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6024470-244B-4C6C-949F-779E1AB78ED3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="2" r:id="rId1"/>
@@ -1047,9 +1047,6 @@
     </r>
   </si>
   <si>
-    <t>Taux de vétusté des construction (en %)</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1296,12 +1293,15 @@
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
     </r>
   </si>
+  <si>
+    <t>Taux de vétusté des constructions (en %)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1362,14 +1362,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1714,14 +1714,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.59765625" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="134.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="134.3984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="279" customHeight="1">
+    <row r="2" spans="1:3" ht="279" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="352.9" customHeight="1">
+    <row r="3" spans="1:3" ht="352.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="317.45" customHeight="1">
+    <row r="4" spans="1:3" ht="317.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1765,71 +1765,71 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="246" customHeight="1">
+    <row r="5" spans="1:3" ht="246" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="46.9">
+    <row r="6" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" ht="46.9">
+    <row r="7" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" ht="197.45" customHeight="1">
+    <row r="8" spans="1:3" ht="197.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.15">
+    <row r="9" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="4"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" ht="31.15">
+    <row r="10" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" ht="31.15">
+    <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" ht="31.15">
+    <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" ht="409.15" customHeight="1">
+    <row r="13" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="298.89999999999998" customHeight="1">
+    <row r="14" spans="1:3" ht="298.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="228" customHeight="1">
+    <row r="15" spans="1:3" ht="228" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
@@ -1862,59 +1862,59 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="409.15" customHeight="1">
+    <row r="16" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="409.15" customHeight="1">
+    <row r="17" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="255" customHeight="1">
+    <row r="18" spans="1:3" ht="255" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="319.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="319.89999999999998" customHeight="1">
-      <c r="A19" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="270.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="270.60000000000002" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>37</v>
+      <c r="C20" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1935,7 +1935,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
(hel-884) Correction du wording sur le taux de vétusté de constructions (#866)
</commit_message>
<xml_diff>
--- a/public/templates/template_comparaison_MS.xlsx
+++ b/public/templates/template_comparaison_MS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\webadm\projets\helios\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://catamaniacrm-my.sharepoint.com/personal/y_elhouakmi_catamania_com/Documents/Documents/DNum/Helios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{F079C0BB-4954-401D-98BD-E461652969BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D29013A-4563-4221-BE0D-8043D3372986}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{F079C0BB-4954-401D-98BD-E461652969BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6024470-244B-4C6C-949F-779E1AB78ED3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="2" r:id="rId1"/>
@@ -1047,9 +1047,6 @@
     </r>
   </si>
   <si>
-    <t>Taux de vétusté des construction (en %)</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1296,12 +1293,15 @@
 Hélios collecte ces données depuis le SI mutualisé des ARS DIAMANT « Décisionnel Inter-ARS pour la Maîtrise et l’Anticipation. », outil décisionnel de pilotage centré sur la régulation de l’offre de soins, abordée sous les aspects des moyens humains, financiers, et productivité.</t>
     </r>
   </si>
+  <si>
+    <t>Taux de vétusté des constructions (en %)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1362,14 +1362,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1714,14 +1714,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18.59765625" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="134.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="134.3984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="279" customHeight="1">
+    <row r="2" spans="1:3" ht="279" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="352.9" customHeight="1">
+    <row r="3" spans="1:3" ht="352.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="317.45" customHeight="1">
+    <row r="4" spans="1:3" ht="317.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -1765,71 +1765,71 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="246" customHeight="1">
+    <row r="5" spans="1:3" ht="246" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="46.9">
+    <row r="6" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" ht="46.9">
+    <row r="7" spans="1:3" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="4"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" ht="197.45" customHeight="1">
+    <row r="8" spans="1:3" ht="197.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.15">
+    <row r="9" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="4"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" ht="31.15">
+    <row r="10" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" ht="31.15">
+    <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:3" ht="31.15">
+    <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" ht="409.15" customHeight="1">
+    <row r="13" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="298.89999999999998" customHeight="1">
+    <row r="14" spans="1:3" ht="298.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="228" customHeight="1">
+    <row r="15" spans="1:3" ht="228" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
@@ -1862,59 +1862,59 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="409.15" customHeight="1">
+    <row r="16" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="409.15" customHeight="1">
+    <row r="17" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="255" customHeight="1">
+    <row r="18" spans="1:3" ht="255" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="319.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="319.89999999999998" customHeight="1">
-      <c r="A19" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="270.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="270.60000000000002" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>37</v>
+      <c r="C20" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1935,7 +1935,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
(hel-964) Ajout du nouvel indicateur
</commit_message>
<xml_diff>
--- a/public/templates/template_comparaison_MS.xlsx
+++ b/public/templates/template_comparaison_MS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://catamaniacrm-my.sharepoint.com/personal/y_elhouakmi_catamania_com/Documents/Documents/DNum/Helios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{F079C0BB-4954-401D-98BD-E461652969BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6024470-244B-4C6C-949F-779E1AB78ED3}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{F079C0BB-4954-401D-98BD-E461652969BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F66F258-AE34-476B-AC09-9369AA712192}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Indicateurs</t>
   </si>
@@ -1295,6 +1295,9 @@
   </si>
   <si>
     <t>Taux de vétusté des constructions (en %)</t>
+  </si>
+  <si>
+    <t>Taux d'occupation global (en %)</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1370,6 +1373,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1710,7 +1716,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587C9ED0-279B-44AC-9485-AC6832055B1B}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1794,7 +1800,7 @@
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -1805,115 +1811,122 @@
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="298.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="228" customHeight="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="298.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="228" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>29</v>
+      <c r="C16" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="255" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:3" ht="255" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="319.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="270.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="319.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="270.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1921,8 +1934,8 @@
   <mergeCells count="4">
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C8:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Hel 964/ajout to global comparaison (#999)
* (hel-964) Ajout du nouvel indicateur

* (hel-964) Update du changelog

* (hel-964) Changement du titre de la modal de detail
</commit_message>
<xml_diff>
--- a/public/templates/template_comparaison_MS.xlsx
+++ b/public/templates/template_comparaison_MS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://catamaniacrm-my.sharepoint.com/personal/y_elhouakmi_catamania_com/Documents/Documents/DNum/Helios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{F079C0BB-4954-401D-98BD-E461652969BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6024470-244B-4C6C-949F-779E1AB78ED3}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{F079C0BB-4954-401D-98BD-E461652969BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F66F258-AE34-476B-AC09-9369AA712192}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Indicateurs</t>
   </si>
@@ -1295,6 +1295,9 @@
   </si>
   <si>
     <t>Taux de vétusté des constructions (en %)</t>
+  </si>
+  <si>
+    <t>Taux d'occupation global (en %)</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1370,6 +1373,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1710,7 +1716,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587C9ED0-279B-44AC-9485-AC6832055B1B}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1794,7 +1800,7 @@
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -1805,115 +1811,122 @@
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="7"/>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="298.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="228" customHeight="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="298.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="228" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>29</v>
+      <c r="C16" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="255" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:3" ht="255" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="319.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="270.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="319.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="270.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1921,8 +1934,8 @@
   <mergeCells count="4">
     <mergeCell ref="C5:C7"/>
     <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C8:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>